<commit_message>
ngfs map data update
see list of updates here: https://app.asana.com/0/0/1204959726561216/f

reference:
L:\Application\Model_One\NextGenFwys\across_runs_union\across_NGF_run_TransitUtilization (6-30 Jose Update).twb

https://app.asana.com/0/1200580945030144/1204492136277500/f
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/metrics/Input Files/NGFS_CorridorMaps_SketchData_v3.xlsx
+++ b/utilities/NextGenFwys/metrics/Input Files/NGFS_CorridorMaps_SketchData_v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atapase\Box\NextGen Freeways Study\07 Tasks\07_AnalysisRound1\Corridor Level Visualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalatorre\Documents\GitHub\travel-model-one\utilities\NextGenFwys\metrics\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA09DEF4-44E4-42E5-BE77-881790A839CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E88F33F-D1E5-41D0-BF6C-68F59D876645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EC2763D9-F6A9-4B72-908C-3B8BAEF8F2AA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{EC2763D9-F6A9-4B72-908C-3B8BAEF8F2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -624,7 +624,7 @@
     <t>4266_4243</t>
   </si>
   <si>
-    <t>8015_1609</t>
+    <t>1609_8015</t>
   </si>
 </sst>
 </file>
@@ -1042,34 +1042,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E935917-F219-4F25-B10A-431E1BE70C9D}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N46" sqref="N46"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1"/>
-    <col min="11" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="72.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.42578125" customWidth="1"/>
-    <col min="16" max="16" width="32.140625" customWidth="1"/>
-    <col min="17" max="17" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="24.26953125" customWidth="1"/>
+    <col min="10" max="10" width="16.26953125" customWidth="1"/>
+    <col min="11" max="13" width="14.7265625" customWidth="1"/>
+    <col min="14" max="14" width="72.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.453125" customWidth="1"/>
+    <col min="16" max="16" width="32.1796875" customWidth="1"/>
+    <col min="17" max="17" width="28.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -2098,10 +2098,10 @@
         <v>1000</v>
       </c>
       <c r="J35" t="s">
+        <v>106</v>
+      </c>
+      <c r="K35" t="s">
         <v>105</v>
-      </c>
-      <c r="K35" t="s">
-        <v>106</v>
       </c>
       <c r="N35" t="s">
         <v>187</v>
@@ -2116,7 +2116,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -2468,59 +2468,59 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D44" s="5"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D45" s="5"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D46" s="5"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D47" s="5"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D48" s="5"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D49" s="5"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D50" s="5"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D51" s="5"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D52" s="5"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D53" s="5"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D54" s="5"/>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D55" s="5"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D56" s="5"/>
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D57" s="5"/>
       <c r="E57" s="3"/>
     </row>
@@ -2539,26 +2539,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA6365E-1C33-4413-9183-AC4217499118}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="42.140625" customWidth="1"/>
+    <col min="5" max="8" width="8.7265625" customWidth="1"/>
+    <col min="9" max="9" width="42.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>6937_6941</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>6941_6937</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>20081_6602</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>6602_20081</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>6484_6590</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>6590_6484</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>6366_6367</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>6367_6366</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>5992_6018</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>6018_5992</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>4195_5651</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>5702_5303</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>4195_5651</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>5702_5303</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>5651_4195</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>5303_5702</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>5651_4195</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>5303_5702</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>4956_4968</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>4968_4956</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>4899_4900</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>5113_5184</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>4900_4899</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>5184_5113</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>4266_	4243</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v xml:space="preserve">	4243_4266</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>4038_12225</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>4072_3990</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>12225_4038</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>3990_4072</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>3532_3492</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>3492_3532</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>2938_	2940</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v xml:space="preserve">	2940_2938</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>3684_	12180</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v xml:space="preserve">	12180_3684</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>2754_2753</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>2753_2754</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>8141_1975</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>1975_	8141</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v xml:space="preserve">	2429_2492</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>2492_	2429</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -4245,13 +4245,13 @@
         <v>28</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E45">
-        <v>12236</v>
+        <v>1625</v>
       </c>
       <c r="F45">
-        <v>1635</v>
+        <v>12234</v>
       </c>
       <c r="G45" t="s">
         <v>155</v>
@@ -4263,17 +4263,17 @@
         <v>187</v>
       </c>
       <c r="J45">
+        <v>1609</v>
+      </c>
+      <c r="K45">
         <v>8015</v>
       </c>
-      <c r="K45" t="s">
-        <v>162</v>
-      </c>
       <c r="L45" t="str">
-        <f t="shared" si="0"/>
-        <v>8015_	1609</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <f>_xlfn.CONCAT(J45,"_",K45)</f>
+        <v>1609_8015</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -4284,13 +4284,13 @@
         <v>28</v>
       </c>
       <c r="D46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E46">
-        <v>1625</v>
+        <v>12236</v>
       </c>
       <c r="F46">
-        <v>12234</v>
+        <v>1635</v>
       </c>
       <c r="G46" t="s">
         <v>156</v>
@@ -4302,17 +4302,17 @@
         <v>187</v>
       </c>
       <c r="J46">
-        <v>1609</v>
-      </c>
-      <c r="K46">
         <v>8015</v>
       </c>
+      <c r="K46" t="s">
+        <v>162</v>
+      </c>
       <c r="L46" t="str">
-        <f t="shared" si="0"/>
-        <v>1609_8015</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <f>_xlfn.CONCAT(J46,"_",K46)</f>
+        <v>8015_	1609</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>29</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>11650_11651</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>11651_11650</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>7910_8182</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -4599,18 +4599,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CD1088-2FC6-40BF-B4A3-2A5937D77DCB}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>181</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -4701,15 +4701,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>126</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>129</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>136</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>131</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>167</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>168</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>169</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>171</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>172</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>171</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>172</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>173</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>174</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>175</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>189</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>176</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>177</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>178</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>190</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>191</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>193</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>182</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>183</v>
       </c>

</xml_diff>

<commit_message>
ngfs maps input data update
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/metrics/Input Files/NGFS_CorridorMaps_SketchData_v3.xlsx
+++ b/utilities/NextGenFwys/metrics/Input Files/NGFS_CorridorMaps_SketchData_v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalatorre\Documents\GitHub\travel-model-one\utilities\NextGenFwys\metrics\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E88F33F-D1E5-41D0-BF6C-68F59D876645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83025B64-9ECD-472E-A590-4EC4F9B21808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{EC2763D9-F6A9-4B72-908C-3B8BAEF8F2AA}"/>
+    <workbookView xWindow="-24120" yWindow="-3765" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="2" xr2:uid="{EC2763D9-F6A9-4B72-908C-3B8BAEF8F2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="199">
   <si>
     <t>Map 1 Inputs: Freeway Corridors AM Peak</t>
   </si>
@@ -625,6 +625,21 @@
   </si>
   <si>
     <t>1609_8015</t>
+  </si>
+  <si>
+    <t>Tasman Dr + Montague Expy + Comstock St + McCarthy Blvd + S Main St</t>
+  </si>
+  <si>
+    <t>5328_5312</t>
+  </si>
+  <si>
+    <t>5709_5674</t>
+  </si>
+  <si>
+    <t>5801_4369</t>
+  </si>
+  <si>
+    <t>5799_5101</t>
   </si>
 </sst>
 </file>
@@ -2537,10 +2552,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA6365E-1C33-4413-9183-AC4217499118}">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2670,7 +2685,7 @@
         <v>6937</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L54" si="0">_xlfn.CONCAT(J4,"_",K4)</f>
+        <f t="shared" ref="L4:L57" si="0">_xlfn.CONCAT(J4,"_",K4)</f>
         <v>6941_6937</v>
       </c>
     </row>
@@ -3012,7 +3027,7 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="J13">
         <v>4195</v>
@@ -3051,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="J14">
         <v>5702</v>
@@ -3090,7 +3105,7 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="J15">
         <v>4195</v>
@@ -3129,7 +3144,7 @@
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="J16">
         <v>5702</v>
@@ -4582,6 +4597,123 @@
       <c r="L54" t="str">
         <f t="shared" si="0"/>
         <v>8182_7910</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" t="s">
+        <v>131</v>
+      </c>
+      <c r="E55">
+        <v>5602</v>
+      </c>
+      <c r="F55">
+        <v>5653</v>
+      </c>
+      <c r="G55" t="s">
+        <v>155</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55" t="s">
+        <v>194</v>
+      </c>
+      <c r="J55">
+        <v>5328</v>
+      </c>
+      <c r="K55">
+        <v>5312</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="0"/>
+        <v>5328_5312</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" t="s">
+        <v>198</v>
+      </c>
+      <c r="E56">
+        <v>5799</v>
+      </c>
+      <c r="F56">
+        <v>5101</v>
+      </c>
+      <c r="G56" t="s">
+        <v>155</v>
+      </c>
+      <c r="H56">
+        <v>3</v>
+      </c>
+      <c r="I56" t="s">
+        <v>194</v>
+      </c>
+      <c r="J56">
+        <v>5709</v>
+      </c>
+      <c r="K56">
+        <v>5674</v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="0"/>
+        <v>5709_5674</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" t="s">
+        <v>198</v>
+      </c>
+      <c r="E57">
+        <v>5799</v>
+      </c>
+      <c r="F57">
+        <v>5101</v>
+      </c>
+      <c r="G57" t="s">
+        <v>155</v>
+      </c>
+      <c r="H57">
+        <v>3</v>
+      </c>
+      <c r="I57" t="s">
+        <v>194</v>
+      </c>
+      <c r="J57">
+        <v>5801</v>
+      </c>
+      <c r="K57">
+        <v>4369</v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="0"/>
+        <v>5801_4369</v>
       </c>
     </row>
   </sheetData>
@@ -4597,10 +4729,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CD1088-2FC6-40BF-B4A3-2A5937D77DCB}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4973,6 +5105,38 @@
         <v>32</v>
       </c>
     </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>196</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>197</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>198</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C45" xr:uid="{90CD1088-2FC6-40BF-B4A3-2A5937D77DCB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>